<commit_message>
First cut devices test
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/devices.xlsx
+++ b/tests/integration_test_files/devices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80BB4BA-16A5-A146-8B61-FFCAA426A94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36639F91-2A04-6B45-9AAD-B9424D710421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="500" windowWidth="48760" windowHeight="27260" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51440" yWindow="500" windowWidth="48760" windowHeight="27260" firstSheet="6" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -28,30 +28,31 @@
     <sheet name="studyDesignTiming" sheetId="12" r:id="rId13"/>
     <sheet name="studyDesignActivities" sheetId="13" r:id="rId14"/>
     <sheet name="studyDesignInterventions" sheetId="14" r:id="rId15"/>
-    <sheet name="studyDevices" sheetId="33" r:id="rId16"/>
-    <sheet name="studyDesignIndications" sheetId="15" r:id="rId17"/>
-    <sheet name="studyDesignPopulations" sheetId="16" r:id="rId18"/>
-    <sheet name="studyDesignCharacteristics" sheetId="17" r:id="rId19"/>
-    <sheet name="studyDesignOE" sheetId="18" r:id="rId20"/>
-    <sheet name="studyDesignEstimands" sheetId="19" r:id="rId21"/>
-    <sheet name="studyDesignProcedures" sheetId="20" r:id="rId22"/>
-    <sheet name="studyDesignEncounters" sheetId="21" r:id="rId23"/>
-    <sheet name="studyDesignElements" sheetId="22" r:id="rId24"/>
-    <sheet name="dictionaries" sheetId="23" r:id="rId25"/>
-    <sheet name="somethingElse" sheetId="24" r:id="rId26"/>
-    <sheet name="spareFormat" sheetId="25" r:id="rId27"/>
-    <sheet name="documentContent" sheetId="27" r:id="rId28"/>
-    <sheet name="people" sheetId="30" r:id="rId29"/>
-    <sheet name="roles" sheetId="29" r:id="rId30"/>
-    <sheet name="studyDesignSites" sheetId="31" r:id="rId31"/>
-    <sheet name="configuration" sheetId="26" r:id="rId32"/>
+    <sheet name="studyDesignProducts" sheetId="34" r:id="rId16"/>
+    <sheet name="studyDevices" sheetId="33" r:id="rId17"/>
+    <sheet name="studyDesignIndications" sheetId="15" r:id="rId18"/>
+    <sheet name="studyDesignPopulations" sheetId="16" r:id="rId19"/>
+    <sheet name="studyDesignCharacteristics" sheetId="17" r:id="rId20"/>
+    <sheet name="studyDesignOE" sheetId="18" r:id="rId21"/>
+    <sheet name="studyDesignEstimands" sheetId="19" r:id="rId22"/>
+    <sheet name="studyDesignProcedures" sheetId="20" r:id="rId23"/>
+    <sheet name="studyDesignEncounters" sheetId="21" r:id="rId24"/>
+    <sheet name="studyDesignElements" sheetId="22" r:id="rId25"/>
+    <sheet name="dictionaries" sheetId="23" r:id="rId26"/>
+    <sheet name="somethingElse" sheetId="24" r:id="rId27"/>
+    <sheet name="spareFormat" sheetId="25" r:id="rId28"/>
+    <sheet name="documentContent" sheetId="27" r:id="rId29"/>
+    <sheet name="people" sheetId="30" r:id="rId30"/>
+    <sheet name="roles" sheetId="29" r:id="rId31"/>
+    <sheet name="studyDesignSites" sheetId="31" r:id="rId32"/>
+    <sheet name="configuration" sheetId="26" r:id="rId33"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="1289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3428" uniqueCount="1330">
   <si>
     <t>name</t>
   </si>
@@ -3913,9 +3914,6 @@
     <t>sourcing</t>
   </si>
   <si>
-    <t>embeddedProduct</t>
-  </si>
-  <si>
     <t>DEVICE1</t>
   </si>
   <si>
@@ -3941,13 +3939,139 @@
   </si>
   <si>
     <t>Locally Sourced</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>administrableDoseForm</t>
+  </si>
+  <si>
+    <t>substanceDescription</t>
+  </si>
+  <si>
+    <t>substanceLabel</t>
+  </si>
+  <si>
+    <t>substanceCode</t>
+  </si>
+  <si>
+    <t>pharmacologicClass</t>
+  </si>
+  <si>
+    <t>productSourcing</t>
+  </si>
+  <si>
+    <t>ingredientRole</t>
+  </si>
+  <si>
+    <t>substanceName</t>
+  </si>
+  <si>
+    <t>strengthName</t>
+  </si>
+  <si>
+    <t>strengthDescription</t>
+  </si>
+  <si>
+    <t>strengthLabel</t>
+  </si>
+  <si>
+    <t>strengthNumerator</t>
+  </si>
+  <si>
+    <t>strengthDenominator</t>
+  </si>
+  <si>
+    <t>referenceSubstanceName</t>
+  </si>
+  <si>
+    <t>referenceSubstanceDescription</t>
+  </si>
+  <si>
+    <t>referenceSubstanceLabel</t>
+  </si>
+  <si>
+    <t>referenceSubstanceCode</t>
+  </si>
+  <si>
+    <t>referenceSubstanceStrengthName</t>
+  </si>
+  <si>
+    <t>referenceSubstanceStrengthDescription</t>
+  </si>
+  <si>
+    <t>referenceSubstanceStrengthLabel</t>
+  </si>
+  <si>
+    <t>referenceSubstanceStrengthNumerator</t>
+  </si>
+  <si>
+    <t>referenceSubstanceStrengthDenominator</t>
+  </si>
+  <si>
+    <t>PROD_1</t>
+  </si>
+  <si>
+    <t>Product 1 Description</t>
+  </si>
+  <si>
+    <t>Brillo Product 1</t>
+  </si>
+  <si>
+    <t>TABLET</t>
+  </si>
+  <si>
+    <t>Centralled Sourced</t>
+  </si>
+  <si>
+    <t>HL7:   100000072072=Active</t>
+  </si>
+  <si>
+    <t>Xano substance</t>
+  </si>
+  <si>
+    <t>Xano</t>
+  </si>
+  <si>
+    <t>FDA: XANO=Xano</t>
+  </si>
+  <si>
+    <t>60MG</t>
+  </si>
+  <si>
+    <t>60 milligram</t>
+  </si>
+  <si>
+    <t>60 mg</t>
+  </si>
+  <si>
+    <t>SUB_XANO</t>
+  </si>
+  <si>
+    <t>SUB_XANO_REF</t>
+  </si>
+  <si>
+    <t>Xano substance reference</t>
+  </si>
+  <si>
+    <t>Xano reference</t>
+  </si>
+  <si>
+    <t>60MG_REF</t>
+  </si>
+  <si>
+    <t>60 milligram ref</t>
+  </si>
+  <si>
+    <t>60 mg reference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4002,8 +4126,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4022,6 +4153,11 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4032,10 +4168,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4190,6 +4327,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -4198,7 +4338,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6682,8 +6823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:H3"/>
+    <sheetView topLeftCell="D1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6729,10 +6870,10 @@
       <c r="F1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="56" t="s">
         <v>358</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="56" t="s">
         <v>359</v>
       </c>
       <c r="I1" s="18" t="s">
@@ -6893,20 +7034,211 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BBE951-9F4A-1B4E-98D1-6D365611D65A}">
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25.5" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" customWidth="1"/>
+    <col min="13" max="13" width="22.83203125" customWidth="1"/>
+    <col min="14" max="14" width="33.33203125" customWidth="1"/>
+    <col min="15" max="15" width="29.1640625" customWidth="1"/>
+    <col min="16" max="16" width="34.83203125" customWidth="1"/>
+    <col min="17" max="17" width="29.33203125" customWidth="1"/>
+    <col min="18" max="18" width="27.83203125" customWidth="1"/>
+    <col min="19" max="19" width="28.5" customWidth="1"/>
+    <col min="20" max="21" width="23.5" customWidth="1"/>
+    <col min="22" max="22" width="31.1640625" customWidth="1"/>
+    <col min="23" max="23" width="36.33203125" customWidth="1"/>
+    <col min="24" max="24" width="31.1640625" customWidth="1"/>
+    <col min="25" max="25" width="40.83203125" customWidth="1"/>
+    <col min="26" max="26" width="31.1640625" customWidth="1"/>
+    <col min="27" max="28" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>1294</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>1295</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>1296</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>1290</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>1291</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>1292</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>1297</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>1298</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>1299</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>1300</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>1301</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>1302</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>1303</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>1304</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>1305</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>1306</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>1307</v>
+      </c>
+      <c r="X1" s="18" t="s">
+        <v>1308</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>1309</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1314</v>
+      </c>
+      <c r="F2" t="s">
+        <v>378</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1315</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1316</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1323</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1317</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1318</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1319</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1320</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1321</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1322</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1324</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1319</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1327</v>
+      </c>
+      <c r="W2" t="s">
+        <v>1328</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D2EF00-74D3-B843-ABED-71D7D63C8B78}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="37" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" style="37" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" style="37" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
     <col min="6" max="6" width="28.33203125" customWidth="1"/>
     <col min="7" max="7" width="40" customWidth="1"/>
   </cols>
@@ -6931,53 +7263,53 @@
         <v>1278</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>1279</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>1280</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>1284</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="36" t="s">
         <v>1281</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="E2" s="36" t="s">
+        <v>1281</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>1282</v>
       </c>
-      <c r="E2" s="36" t="s">
-        <v>1282</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>1283</v>
-      </c>
       <c r="G2" s="11" t="s">
-        <v>371</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>1285</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>1286</v>
-      </c>
       <c r="C3" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>563</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F3" t="s">
         <v>1287</v>
       </c>
-      <c r="F3" t="s">
-        <v>1288</v>
-      </c>
-      <c r="G3" t="s">
-        <v>389</v>
+      <c r="G3" s="11" t="s">
+        <v>1311</v>
       </c>
     </row>
   </sheetData>
@@ -6985,7 +7317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -7048,7 +7380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -7162,72 +7494,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>418</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>422</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>422</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>421</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>424</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>424</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>425</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7302,6 +7568,72 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>422</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>422</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>425</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
@@ -7713,7 +8045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -7770,7 +8102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -7861,7 +8193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -8171,7 +8503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -8315,7 +8647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -8435,7 +8767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:F135"/>
   <sheetViews>
@@ -11131,7 +11463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:F133"/>
   <sheetViews>
@@ -13814,7 +14146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250E6F23-B764-5243-842F-046C5535819A}">
   <dimension ref="A1:B134"/>
   <sheetViews>
@@ -14538,57 +14870,6 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62A79FA-4693-DC4C-8533-78F85FC1D1D4}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>1236</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1259</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1238</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1257</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>1244</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -14714,6 +14995,57 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62A79FA-4693-DC4C-8533-78F85FC1D1D4}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>1236</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F6DEFA-A517-8846-A522-4BE1FE1D8CBC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -14797,7 +15129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B0C263-3963-0B49-B113-94AC2CB14316}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -14885,7 +15217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -15029,120 +15361,120 @@
       <c r="A1" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
     </row>
     <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add in product roles
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/devices.xlsx
+++ b/tests/integration_test_files/devices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E5AFBE-56DE-5442-BA8B-5D1A2491130D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D9DD14-BEA0-D148-B3AE-31C1EC5430DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51440" yWindow="500" windowWidth="48760" windowHeight="27260" firstSheet="6" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="62200" yWindow="11380" windowWidth="37960" windowHeight="16380" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -30,29 +30,30 @@
     <sheet name="studyDesignInterventions" sheetId="14" r:id="rId15"/>
     <sheet name="studyDesignProducts" sheetId="34" r:id="rId16"/>
     <sheet name="studyDevices" sheetId="33" r:id="rId17"/>
-    <sheet name="studyDesignIndications" sheetId="15" r:id="rId18"/>
-    <sheet name="studyDesignPopulations" sheetId="16" r:id="rId19"/>
-    <sheet name="studyDesignCharacteristics" sheetId="17" r:id="rId20"/>
-    <sheet name="studyDesignOE" sheetId="18" r:id="rId21"/>
-    <sheet name="studyDesignEstimands" sheetId="19" r:id="rId22"/>
-    <sheet name="studyDesignProcedures" sheetId="20" r:id="rId23"/>
-    <sheet name="studyDesignEncounters" sheetId="21" r:id="rId24"/>
-    <sheet name="studyDesignElements" sheetId="22" r:id="rId25"/>
-    <sheet name="dictionaries" sheetId="23" r:id="rId26"/>
-    <sheet name="somethingElse" sheetId="24" r:id="rId27"/>
-    <sheet name="spareFormat" sheetId="25" r:id="rId28"/>
-    <sheet name="documentContent" sheetId="27" r:id="rId29"/>
-    <sheet name="people" sheetId="30" r:id="rId30"/>
-    <sheet name="roles" sheetId="29" r:id="rId31"/>
-    <sheet name="studyDesignSites" sheetId="31" r:id="rId32"/>
-    <sheet name="configuration" sheetId="26" r:id="rId33"/>
+    <sheet name="deviceRoles" sheetId="35" r:id="rId18"/>
+    <sheet name="studyDesignIndications" sheetId="15" r:id="rId19"/>
+    <sheet name="studyDesignPopulations" sheetId="16" r:id="rId20"/>
+    <sheet name="studyDesignCharacteristics" sheetId="17" r:id="rId21"/>
+    <sheet name="studyDesignOE" sheetId="18" r:id="rId22"/>
+    <sheet name="studyDesignEstimands" sheetId="19" r:id="rId23"/>
+    <sheet name="studyDesignProcedures" sheetId="20" r:id="rId24"/>
+    <sheet name="studyDesignEncounters" sheetId="21" r:id="rId25"/>
+    <sheet name="studyDesignElements" sheetId="22" r:id="rId26"/>
+    <sheet name="dictionaries" sheetId="23" r:id="rId27"/>
+    <sheet name="somethingElse" sheetId="24" r:id="rId28"/>
+    <sheet name="spareFormat" sheetId="25" r:id="rId29"/>
+    <sheet name="documentContent" sheetId="27" r:id="rId30"/>
+    <sheet name="people" sheetId="30" r:id="rId31"/>
+    <sheet name="roles" sheetId="29" r:id="rId32"/>
+    <sheet name="studyDesignSites" sheetId="31" r:id="rId33"/>
+    <sheet name="configuration" sheetId="26" r:id="rId34"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3428" uniqueCount="1329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3440" uniqueCount="1334">
   <si>
     <t>name</t>
   </si>
@@ -4062,6 +4063,21 @@
   </si>
   <si>
     <t>60 mg reference</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>appliesTo</t>
+  </si>
+  <si>
+    <t>DEVICE_ROLE_1</t>
+  </si>
+  <si>
+    <t>Device Role 1</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
   </si>
 </sst>
 </file>
@@ -7034,7 +7050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BBE951-9F4A-1B4E-98D1-6D365611D65A}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -7225,9 +7241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D2EF00-74D3-B843-ABED-71D7D63C8B78}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7315,6 +7329,68 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BA0B96-DF59-C94B-9DB9-AD5C769114C4}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1270</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -7369,123 +7445,6 @@
       </c>
       <c r="D3" s="8" t="s">
         <v>404</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="53.5" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>405</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>406</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>407</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>408</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>411</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="E2" s="3">
-        <v>300</v>
-      </c>
-      <c r="F2" s="3">
-        <v>300</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>415</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="I3" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>415</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="I4" t="s">
-        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -7565,6 +7524,123 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+    <col min="3" max="3" width="53.5" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="E2" s="3">
+        <v>300</v>
+      </c>
+      <c r="F2" s="3">
+        <v>300</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="I3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="I4" t="s">
+        <v>421</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -7630,7 +7706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
@@ -8042,7 +8118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -8099,7 +8175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -8190,7 +8266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -8500,7 +8576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -8644,7 +8720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -8764,7 +8840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:F135"/>
   <sheetViews>
@@ -11460,7 +11536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:F133"/>
   <sheetViews>
@@ -14133,733 +14209,6 @@
         <v>49</v>
       </c>
       <c r="F133" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250E6F23-B764-5243-842F-046C5535819A}">
-  <dimension ref="A1:B134"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A133" sqref="A2:A133"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="115.83203125" style="6" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>969</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
-        <v>973</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="36" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>978</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
-        <v>980</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>982</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
-        <v>983</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="36" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="36" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="36" t="s">
-        <v>989</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36" t="s">
-        <v>991</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>992</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="36" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36" t="s">
-        <v>995</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="36" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="36" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="36" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="36" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="36" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="36" t="s">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="36" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="36" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="181" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>1012</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="36" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="36" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="36" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="36" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="36" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="11" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="36" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="11" t="s">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="36" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="11" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="36" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="11" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="36" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="11" t="s">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="36" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="11" t="s">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="36" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="11" t="s">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="36" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="11" t="s">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="36" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="11" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="36" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="11" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="36" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="11" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="36" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="11" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="36" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="11" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="36" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="11" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="36" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="11" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="36" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="11" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="36" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="11" t="s">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="36" t="s">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="11" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="36" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="11" t="s">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="36" t="s">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="11" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="36" t="s">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="11" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="36" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="11" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="36" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="11" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="36" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="11" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="36" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="11" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="36" t="s">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="11" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="36" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="11" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="36" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="11" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="36" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="11" t="s">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="36" t="s">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="11" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="36" t="s">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="11" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="36" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="11" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="36" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="11" t="s">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="36" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="11" t="s">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="36" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="11" t="s">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="36" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="11" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="36" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="11" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="36" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="11" t="s">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="36" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="11" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="36" t="s">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="11" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134" s="11" t="s">
         <v>1101</v>
       </c>
     </row>
@@ -14992,6 +14341,733 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250E6F23-B764-5243-842F-046C5535819A}">
+  <dimension ref="A1:B134"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A133" sqref="A2:A133"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="115.83203125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>969</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
+        <v>973</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="36" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>978</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>980</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>982</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="36" t="s">
+        <v>983</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="36" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="36" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="36" t="s">
+        <v>989</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="36" t="s">
+        <v>991</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>992</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="36" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="36" t="s">
+        <v>995</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="36" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="36" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="36" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="36" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="36" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="36" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="36" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="36" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="181" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="36" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="36" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="36" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="36" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="36" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="36" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="36" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="36" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="36" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="36" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="36" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="11" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="36" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="36" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="11" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="36" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="11" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="36" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="11" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="36" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="11" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="36" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="11" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="36" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="11" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="36" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="11" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="36" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="11" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="36" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="11" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="36" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="11" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="36" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="11" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="36" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="36" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="11" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="36" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="11" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="36" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="11" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="36" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="11" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="36" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="11" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="36" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="11" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="36" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="11" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="36" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="11" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="36" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="11" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="36" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="11" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="36" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="11" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="36" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="11" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="36" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="11" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="36" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="11" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="36" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="11" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="36" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="11" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="36" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="11" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="36" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="11" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="36" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="11" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="36" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="11" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="11" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62A79FA-4693-DC4C-8533-78F85FC1D1D4}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -15042,7 +15118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F6DEFA-A517-8846-A522-4BE1FE1D8CBC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -15126,7 +15202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B0C263-3963-0B49-B113-94AC2CB14316}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -15214,7 +15290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>

</xml_diff>

<commit_message>
RangeQuantity change, DDF-RA #630
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/devices.xlsx
+++ b/tests/integration_test_files/devices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC2C901-AFD6-1740-985E-4964F322996B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4A2F0D-1E7B-E94F-9B06-B8B21480C567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="45680" windowHeight="27220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="45680" windowHeight="27220" firstSheet="19" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3446" uniqueCount="1334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3449" uniqueCount="1337">
   <si>
     <t>name</t>
   </si>
@@ -4078,6 +4078,15 @@
   </si>
   <si>
     <t>AMEND_1</t>
+  </si>
+  <si>
+    <t>1 mg</t>
+  </si>
+  <si>
+    <t>10mg</t>
+  </si>
+  <si>
+    <t>1 liter</t>
   </si>
 </sst>
 </file>
@@ -7037,8 +7046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BBE951-9F4A-1B4E-98D1-6D365611D65A}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="L1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7067,7 +7076,7 @@
     <col min="23" max="23" width="36.33203125" customWidth="1"/>
     <col min="24" max="24" width="31.1640625" customWidth="1"/>
     <col min="25" max="25" width="40.83203125" customWidth="1"/>
-    <col min="26" max="26" width="31.1640625" customWidth="1"/>
+    <col min="26" max="26" width="39.6640625" customWidth="1"/>
     <col min="27" max="28" width="36" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7197,6 +7206,12 @@
       <c r="O2" t="s">
         <v>1318</v>
       </c>
+      <c r="P2" t="s">
+        <v>1334</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1336</v>
+      </c>
       <c r="R2" t="s">
         <v>1320</v>
       </c>
@@ -7217,6 +7232,9 @@
       </c>
       <c r="X2" t="s">
         <v>1325</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>1335</v>
       </c>
     </row>
   </sheetData>
@@ -7446,7 +7464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -14347,14 +14365,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250E6F23-B764-5243-842F-046C5535819A}">
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A133" sqref="A2:A133"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="115.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="182.33203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated files for personName including tests
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/devices.xlsx
+++ b/tests/integration_test_files/devices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4A2F0D-1E7B-E94F-9B06-B8B21480C567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AF943C-4572-8B4E-8BB0-A3BF070B4E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="45680" windowHeight="27220" firstSheet="19" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17380" firstSheet="23" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3449" uniqueCount="1337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3451" uniqueCount="1339">
   <si>
     <t>name</t>
   </si>
@@ -4087,6 +4087,12 @@
   </si>
   <si>
     <t>1 liter</t>
+  </si>
+  <si>
+    <t>personName</t>
+  </si>
+  <si>
+    <t>, Fred, Smith,</t>
   </si>
 </sst>
 </file>
@@ -14365,7 +14371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250E6F23-B764-5243-842F-046C5535819A}">
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -15090,10 +15096,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62A79FA-4693-DC4C-8533-78F85FC1D1D4}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15101,9 +15107,10 @@
     <col min="1" max="3" width="15.83203125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -15119,8 +15126,11 @@
       <c r="E1" s="18" t="s">
         <v>1234</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="18" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1256</v>
       </c>
@@ -15132,6 +15142,9 @@
       </c>
       <c r="E2" s="3" t="s">
         <v>1241</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>